<commit_message>
Automatische test-sync: 2025-08-03 02:12:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -738,8 +738,64 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Testmail #1: Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Beste klant, 
+Bedankt voor uw e-mail. Om u zo goed mogelijk van dienst te kunnen zijn, ontvang ik graag meer informatie over wat u precies geregeld wilt hebben. Kunt u mij wat meer details geven, zodat ik u beter kan helpen? Alvast bedankt voor uw medewerking.
+Met vriendelijke groet, 
+[Naam]
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-08-03 02:12:12</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2">
+  <conditionalFormatting sqref="D2:D3">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -759,7 +815,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2">
+  <conditionalFormatting sqref="G2:G3">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -767,17 +823,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2">
+  <conditionalFormatting sqref="H2:H3">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2">
+  <conditionalFormatting sqref="I2:I3">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2">
+  <conditionalFormatting sqref="J2:J3">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -819,7 +875,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 02:21:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -794,8 +794,63 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Testmail #1: Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw e-mail. Om u beter van dienst te kunnen zijn, heb ik meer informatie nodig over wat u precies geregeld wilt hebben. Kunt u alstublieft wat meer details geven of specifiëren waar u hulp bij nodig heeft? Zodra ik meer informatie heb, zal ik ervoor zorgen dat dit zo spoedig mogelijk voor u wordt geregeld.
+Met vriendelijke groet,
+[E-mailassistent]</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-08-03 02:21:09</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D3">
+  <conditionalFormatting sqref="D2:D4">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -815,7 +870,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G3">
+  <conditionalFormatting sqref="G2:G4">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -823,17 +878,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H3">
+  <conditionalFormatting sqref="H2:H4">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I3">
+  <conditionalFormatting sqref="I2:I4">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J3">
+  <conditionalFormatting sqref="J2:J4">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -875,7 +930,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 13:41:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -849,8 +849,64 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Testmail #1: Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Geachte klant,
+Dank u wel voor uw bericht. Om u zo goed mogelijk van dienst te kunnen zijn, zou ik graag meer details willen ontvangen over wat u precies geregeld wilt hebben. Kunt u alstublieft specifiëren welke specifieke taak u uitgevoerd wilt hebben?
+Met vriendelijke groet,
+[Naam] 
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2025-08-03 13:40:54</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D4">
+  <conditionalFormatting sqref="D2:D5">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -870,7 +926,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G4">
+  <conditionalFormatting sqref="G2:G5">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -878,17 +934,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H4">
+  <conditionalFormatting sqref="H2:H5">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I4">
+  <conditionalFormatting sqref="I2:I5">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J4">
+  <conditionalFormatting sqref="J2:J5">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -930,7 +986,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 14:06:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -905,8 +905,63 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Testmail #1: Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw bericht. Om u beter van dienst te kunnen zijn, hebben wij meer details nodig over wat precies geregeld moet worden. Kunt u specifiek aangeven waarover u hulp nodig heeft?
+Met vriendelijke groet,
+[Naam bedrijf] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2025-08-03 14:06:05</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D5">
+  <conditionalFormatting sqref="D2:D6">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -926,7 +981,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G5">
+  <conditionalFormatting sqref="G2:G6">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -934,17 +989,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H5">
+  <conditionalFormatting sqref="H2:H6">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I5">
+  <conditionalFormatting sqref="I2:I6">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J5">
+  <conditionalFormatting sqref="J2:J6">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -986,7 +1041,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 14:13:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -960,8 +960,60 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Testmail #1: Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar support@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2025-08-03 14:12:56</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D6">
+  <conditionalFormatting sqref="D2:D7">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -981,7 +1033,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G6">
+  <conditionalFormatting sqref="G2:G7">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -989,17 +1041,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H6">
+  <conditionalFormatting sqref="H2:H7">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I6">
+  <conditionalFormatting sqref="I2:I7">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J6">
+  <conditionalFormatting sqref="J2:J7">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1041,7 +1093,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 14:20:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2</f>
+              <f>'Dashboard'!$A$2:$A$3</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2</f>
+              <f>'Dashboard'!$B$2:$B$3</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1012,8 +1012,60 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Testmail #1: Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2025-08-03 14:19:58</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D7">
+  <conditionalFormatting sqref="D2:D8">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1033,7 +1085,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G7">
+  <conditionalFormatting sqref="G2:G8">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1041,17 +1093,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H7">
+  <conditionalFormatting sqref="H2:H8">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I7">
+  <conditionalFormatting sqref="I2:I8">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J7">
+  <conditionalFormatting sqref="J2:J8">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1066,7 +1118,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1096,6 +1148,16 @@
         <v>6</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 14:22:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$3</f>
+              <f>'Dashboard'!$A$2:$A$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$3</f>
+              <f>'Dashboard'!$B$2:$B$4</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1064,8 +1064,63 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Wil je dit oppakken?</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Testmail #2: Wil je dit oppakken?</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Beste afzender,
+Bedankt voor je bericht. Kun je specifieker zijn over het onderwerp dat je graag wilt dat er wordt opgepakt? Als je meer details kunt geven, kan ik je beter helpen. 
+Met vriendelijke groet,
+[Naam bedrijf] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2025-08-03 14:22:08</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D8">
+  <conditionalFormatting sqref="D2:D9">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1085,7 +1140,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G8">
+  <conditionalFormatting sqref="G2:G9">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1093,17 +1148,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H8">
+  <conditionalFormatting sqref="H2:H9">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I8">
+  <conditionalFormatting sqref="I2:I9">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J8">
+  <conditionalFormatting sqref="J2:J9">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1118,7 +1173,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1158,6 +1213,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 14:26:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1119,8 +1119,60 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Testmail #1: Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2025-08-03 14:26:46</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D9">
+  <conditionalFormatting sqref="D2:D10">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1140,7 +1192,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G9">
+  <conditionalFormatting sqref="G2:G10">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1148,17 +1200,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H9">
+  <conditionalFormatting sqref="H2:H10">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I9">
+  <conditionalFormatting sqref="I2:I10">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J9">
+  <conditionalFormatting sqref="J2:J10">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1210,7 +1262,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 14:29:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1171,8 +1171,64 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Wil je dit oppakken?</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Testmail #2: Wil je dit oppakken?</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Geachte afzender,
+Dank u voor uw e-mail. Kunt u wat meer context geven over wat u precies bedoelt met "Testmail #2: Wil je dit oppakken"? Zo kan ik u beter van dienst zijn. 
+Met vriendelijke groet,
+[Naam]
+Nederlandse e-mailassistent</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2025-08-03 14:28:55</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D10">
+  <conditionalFormatting sqref="D2:D11">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1192,7 +1248,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G10">
+  <conditionalFormatting sqref="G2:G11">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1200,17 +1256,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H10">
+  <conditionalFormatting sqref="H2:H11">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I10">
+  <conditionalFormatting sqref="I2:I11">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J10">
+  <conditionalFormatting sqref="J2:J11">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1272,7 +1328,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 14:33:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1227,8 +1227,60 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Testmail #1: Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2025-08-03 14:33:46</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D11">
+  <conditionalFormatting sqref="D2:D12">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1248,7 +1300,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G11">
+  <conditionalFormatting sqref="G2:G12">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1256,17 +1308,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H11">
+  <conditionalFormatting sqref="H2:H12">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I11">
+  <conditionalFormatting sqref="I2:I12">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J11">
+  <conditionalFormatting sqref="J2:J12">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1318,7 +1370,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 14:36:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1279,8 +1279,60 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Wil je dit oppakken?</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Testmail #2: Wil je dit oppakken?</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar support@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2025-08-03 14:35:56</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D12">
+  <conditionalFormatting sqref="D2:D13">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1300,7 +1352,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G12">
+  <conditionalFormatting sqref="G2:G13">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1308,17 +1360,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H12">
+  <conditionalFormatting sqref="H2:H13">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I12">
+  <conditionalFormatting sqref="I2:I13">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J12">
+  <conditionalFormatting sqref="J2:J13">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1380,7 +1432,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 14:38:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1331,8 +1331,60 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Kun jij dit afhandelen?</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Testmail #3: Kun jij dit afhandelen?</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2025-08-03 14:38:07</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D13">
+  <conditionalFormatting sqref="D2:D14">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1352,7 +1404,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G13">
+  <conditionalFormatting sqref="G2:G14">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1360,17 +1412,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H13">
+  <conditionalFormatting sqref="H2:H14">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I13">
+  <conditionalFormatting sqref="I2:I14">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J13">
+  <conditionalFormatting sqref="J2:J14">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1422,7 +1474,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 14:42:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1383,8 +1383,63 @@
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Wil je deze klant bellen?</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Testmail #5: Wil je deze klant bellen?</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Geachte klantenservice,
+Dit is slechts een testmail om te controleren of het systeem werkt. Er is geen echte klant die gebeld hoeft te worden.
+Met vriendelijke groet,
+[Naam]</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2025-08-03 14:42:28</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D14">
+  <conditionalFormatting sqref="D2:D15">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1404,7 +1459,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G14">
+  <conditionalFormatting sqref="G2:G15">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1412,17 +1467,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H14">
+  <conditionalFormatting sqref="H2:H15">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I14">
+  <conditionalFormatting sqref="I2:I15">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J14">
+  <conditionalFormatting sqref="J2:J15">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1484,7 +1539,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 14:44:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$4</f>
+              <f>'Dashboard'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$4</f>
+              <f>'Dashboard'!$B$2:$B$5</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1438,8 +1438,60 @@
         </is>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Hebben we EcoPro-700 nog op voorraad?</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Testmail #6: Hebben we EcoPro-700 nog op voorraad?</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Inkoop / Bestellingen</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar inkoop@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2025-08-03 14:44:39</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D15">
+  <conditionalFormatting sqref="D2:D16">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1459,7 +1511,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G15">
+  <conditionalFormatting sqref="G2:G16">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1467,17 +1519,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H15">
+  <conditionalFormatting sqref="H2:H16">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I15">
+  <conditionalFormatting sqref="I2:I16">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J15">
+  <conditionalFormatting sqref="J2:J16">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1492,7 +1544,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1542,6 +1594,16 @@
         <v>4</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Inkoop / Bestellingen</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 14:47:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1490,8 +1490,60 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Is dit artikel nog op voorraad?</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Testmail #7: Is dit artikel nog op voorraad?</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Inkoop / Bestellingen</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar inkoop@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2025-08-03 14:46:50</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D16">
+  <conditionalFormatting sqref="D2:D17">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1511,7 +1563,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G16">
+  <conditionalFormatting sqref="G2:G17">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1519,17 +1571,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H16">
+  <conditionalFormatting sqref="H2:H17">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I16">
+  <conditionalFormatting sqref="I2:I17">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J16">
+  <conditionalFormatting sqref="J2:J17">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1601,7 +1653,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 14:49:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1542,8 +1542,60 @@
         </is>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Kun je nagaan of dit nog leverbaar is?</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Testmail #8: Kun je nagaan of dit nog leverbaar is?</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Inkoop / Bestellingen</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar inkoop@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2025-08-03 14:49:01</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D17">
+  <conditionalFormatting sqref="D2:D18">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1563,7 +1615,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G17">
+  <conditionalFormatting sqref="G2:G18">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1571,17 +1623,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H17">
+  <conditionalFormatting sqref="H2:H18">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I17">
+  <conditionalFormatting sqref="I2:I18">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J17">
+  <conditionalFormatting sqref="J2:J18">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1653,7 +1705,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 14:51:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1594,8 +1594,63 @@
         </is>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Hoi, hebben jullie al iets gehoord?</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Testmail #9: Hoi, hebben jullie al iets gehoord?</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw e-mail. Kunt u ons meer informatie geven over waar u precies op wacht of waar u over gehoord wilt hebben? Zo kunnen wij u beter van dienst zijn.
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2025-08-03 14:51:12</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D18">
+  <conditionalFormatting sqref="D2:D19">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1615,7 +1670,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G18">
+  <conditionalFormatting sqref="G2:G19">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1623,17 +1678,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H18">
+  <conditionalFormatting sqref="H2:H19">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I18">
+  <conditionalFormatting sqref="I2:I19">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J18">
+  <conditionalFormatting sqref="J2:J19">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1681,17 +1736,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Planning / Afspraak</t>
+          <t>Overig</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Overig</t>
+          <t>Planning / Afspraak</t>
         </is>
       </c>
       <c r="B4" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 14:53:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1649,8 +1649,63 @@
         </is>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Is er al nieuws?</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Testmail #10: Is er al nieuws?</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Beste afzender,
+Bedankt voor je e-mail. Om je vraag te beantwoorden hebben we wat meer context nodig. Zou je kunnen aangeven waarover je precies nieuws verwacht? Zo kunnen we je beter van dienst zijn.
+Met vriendelijke groet,
+[Naam bedrijf] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2025-08-03 14:53:24</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D19">
+  <conditionalFormatting sqref="D2:D20">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1670,7 +1725,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G19">
+  <conditionalFormatting sqref="G2:G20">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1678,17 +1733,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H19">
+  <conditionalFormatting sqref="H2:H20">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I19">
+  <conditionalFormatting sqref="I2:I20">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J19">
+  <conditionalFormatting sqref="J2:J20">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1740,7 +1795,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 15:00:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$5</f>
+              <f>'Dashboard'!$A$2:$A$6</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$5</f>
+              <f>'Dashboard'!$B$2:$B$6</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1704,8 +1704,60 @@
         </is>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Kun je mij de datasheet van de VentiQ-250 sturen?</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Testmail #13: Kun je mij de datasheet van de VentiQ-250 sturen?</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Documentatie / Datasheets</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar documentatie@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2025-08-03 14:59:51</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D20">
+  <conditionalFormatting sqref="D2:D21">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1725,7 +1777,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G20">
+  <conditionalFormatting sqref="G2:G21">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1733,17 +1785,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H20">
+  <conditionalFormatting sqref="H2:H21">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I20">
+  <conditionalFormatting sqref="I2:I21">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J20">
+  <conditionalFormatting sqref="J2:J21">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1758,7 +1810,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1818,6 +1870,16 @@
         <v>3</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Documentatie / Datasheets</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 15:02:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1756,8 +1756,60 @@
         </is>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Heb je de CE-certificaten van dit product?</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Testmail #14: Heb je de CE-certificaten van dit product?</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar support@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2025-08-03 15:02:02</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D21">
+  <conditionalFormatting sqref="D2:D22">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1777,7 +1829,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G21">
+  <conditionalFormatting sqref="G2:G22">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1785,17 +1837,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H21">
+  <conditionalFormatting sqref="H2:H22">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I21">
+  <conditionalFormatting sqref="I2:I22">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J21">
+  <conditionalFormatting sqref="J2:J22">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1833,17 +1885,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Intern verzoek / Actie voor medewerker</t>
+          <t>Overig</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Overig</t>
+          <t>Intern verzoek / Actie voor medewerker</t>
         </is>
       </c>
       <c r="B3" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 15:04:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1808,8 +1808,60 @@
         </is>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Leg dit even neer bij Koen.</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Testmail #15: Leg dit even neer bij Koen.</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>2025-08-03 15:04:15</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D22">
+  <conditionalFormatting sqref="D2:D23">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1829,7 +1881,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G22">
+  <conditionalFormatting sqref="G2:G23">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1837,17 +1889,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H22">
+  <conditionalFormatting sqref="H2:H23">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I22">
+  <conditionalFormatting sqref="I2:I23">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J22">
+  <conditionalFormatting sqref="J2:J23">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1909,7 +1961,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 15:06:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1860,8 +1860,60 @@
         </is>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Wil je dit even doorsturen?</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Testmail #16: Wil je dit even doorsturen?</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar support@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>2025-08-03 15:06:27</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D23">
+  <conditionalFormatting sqref="D2:D24">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1881,7 +1933,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G23">
+  <conditionalFormatting sqref="G2:G24">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1889,17 +1941,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H23">
+  <conditionalFormatting sqref="H2:H24">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I23">
+  <conditionalFormatting sqref="I2:I24">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J23">
+  <conditionalFormatting sqref="J2:J24">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1941,7 +1993,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 15:08:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1912,8 +1912,60 @@
         </is>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Testmail #17: Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>2025-08-03 15:08:38</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D24">
+  <conditionalFormatting sqref="D2:D25">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1933,7 +1985,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G24">
+  <conditionalFormatting sqref="G2:G25">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1941,17 +1993,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H24">
+  <conditionalFormatting sqref="H2:H25">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I24">
+  <conditionalFormatting sqref="I2:I25">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J24">
+  <conditionalFormatting sqref="J2:J25">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2013,7 +2065,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 15:10:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1964,8 +1964,60 @@
         </is>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Bestel je 200 stuks M8-bouten RVS voor Van Dijk?</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Testmail #18: Bestel je 200 stuks M8-bouten RVS voor Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Inkoop / Bestellingen</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar inkoop@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>2025-08-03 15:10:49</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D25">
+  <conditionalFormatting sqref="D2:D26">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1985,7 +2037,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G25">
+  <conditionalFormatting sqref="G2:G26">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1993,17 +2045,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H25">
+  <conditionalFormatting sqref="H2:H26">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I25">
+  <conditionalFormatting sqref="I2:I26">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J25">
+  <conditionalFormatting sqref="J2:J26">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2075,7 +2127,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 15:13:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2016,8 +2016,64 @@
         </is>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Bel jij klant Jansen even?</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Testmail #19: Bel jij klant Jansen even?</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Geachte heer/mevrouw,
+Dank voor uw bericht. Om u verder te kunnen helpen, ontvang ik graag meer informatie. Kunt u aangeven waarom klant Jansen gebeld dient te worden en welk specifiek onderwerp dit betreft? Zo kan ik ervoor zorgen dat de juiste persoon of afdeling contact met hem opneemt.
+Met vriendelijke groet,
+[Naam]
+E-mailassistent van [Bedrijfsnaam]</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>2025-08-03 15:13:02</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D26">
+  <conditionalFormatting sqref="D2:D27">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2037,7 +2093,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G26">
+  <conditionalFormatting sqref="G2:G27">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2045,17 +2101,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H26">
+  <conditionalFormatting sqref="H2:H27">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I26">
+  <conditionalFormatting sqref="I2:I27">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J26">
+  <conditionalFormatting sqref="J2:J27">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2097,7 +2153,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 15:15:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$6</f>
+              <f>'Dashboard'!$A$2:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$6</f>
+              <f>'Dashboard'!$B$2:$B$7</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2072,8 +2072,60 @@
         </is>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Ik ben niet tevreden over hoe dit is gegaan.</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Testmail #20: Ik ben niet tevreden over hoe dit is gegaan.</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Klacht / Probleem</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar klachten@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>2025-08-03 15:15:14</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D27">
+  <conditionalFormatting sqref="D2:D28">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2093,7 +2145,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G27">
+  <conditionalFormatting sqref="G2:G28">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2101,17 +2153,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H27">
+  <conditionalFormatting sqref="H2:H28">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I27">
+  <conditionalFormatting sqref="I2:I28">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J27">
+  <conditionalFormatting sqref="J2:J28">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2126,7 +2178,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2196,6 +2248,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Klacht / Probleem</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 18:12:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2124,8 +2124,60 @@
         </is>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Testmail #1: Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>2025-08-03 18:12:40</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D28">
+  <conditionalFormatting sqref="D2:D29">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2145,7 +2197,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G28">
+  <conditionalFormatting sqref="G2:G29">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2153,17 +2205,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H28">
+  <conditionalFormatting sqref="H2:H29">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I28">
+  <conditionalFormatting sqref="I2:I29">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J28">
+  <conditionalFormatting sqref="J2:J29">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2211,17 +2263,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Intern verzoek / Actie voor medewerker</t>
+          <t>Planning / Afspraak</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Planning / Afspraak</t>
+          <t>Intern verzoek / Actie voor medewerker</t>
         </is>
       </c>
       <c r="B4" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 18:15:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2176,8 +2176,60 @@
         </is>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Wil je dit oppakken?</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Testmail #2: Wil je dit oppakken?</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>2025-08-03 18:14:51</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D29">
+  <conditionalFormatting sqref="D2:D30">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2197,7 +2249,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G29">
+  <conditionalFormatting sqref="G2:G30">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2205,17 +2257,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H29">
+  <conditionalFormatting sqref="H2:H30">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I29">
+  <conditionalFormatting sqref="I2:I30">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J29">
+  <conditionalFormatting sqref="J2:J30">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2267,7 +2319,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 18:17:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2228,8 +2228,60 @@
         </is>
       </c>
     </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Kun jij dit afhandelen?</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Testmail #3: Kun jij dit afhandelen?</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>2025-08-03 18:17:02</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D30">
+  <conditionalFormatting sqref="D2:D31">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2249,7 +2301,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G30">
+  <conditionalFormatting sqref="G2:G31">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2257,17 +2309,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H30">
+  <conditionalFormatting sqref="H2:H31">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I30">
+  <conditionalFormatting sqref="I2:I31">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J30">
+  <conditionalFormatting sqref="J2:J31">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2305,7 +2357,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Overig</t>
+          <t>Planning / Afspraak</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -2315,11 +2367,11 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Planning / Afspraak</t>
+          <t>Overig</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 18:19:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2280,8 +2280,63 @@
         </is>
       </c>
     </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Wil je 100 stuks M5-bouten bestellen?</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Testmail #4: Wil je 100 stuks M5-bouten bestellen?</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Inkoop / Bestellingen</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Hartelijk dank voor je interesse in onze producten. Helaas kan ik je niet helpen met deze specifieke bestelling via e-mail. Voor het plaatsen van een bestelling verwijs ik je graag door naar onze website of klantenservice. Mocht je hulp nodig hebben bij het plaatsen van een bestelling, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Naam bedrijf] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>2025-08-03 18:19:13</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D31">
+  <conditionalFormatting sqref="D2:D32">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2301,7 +2356,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G31">
+  <conditionalFormatting sqref="G2:G32">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2309,17 +2364,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H31">
+  <conditionalFormatting sqref="H2:H32">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I31">
+  <conditionalFormatting sqref="I2:I32">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J31">
+  <conditionalFormatting sqref="J2:J32">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2391,7 +2446,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 18:21:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$7</f>
+              <f>'Dashboard'!$A$2:$A$8</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$7</f>
+              <f>'Dashboard'!$B$2:$B$8</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2335,8 +2335,60 @@
         </is>
       </c>
     </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Wil je deze klant bellen?</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Testmail #5: Wil je deze klant bellen?</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Klantenservice / Contact</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar klantenservice@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>2025-08-03 18:21:26</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D32">
+  <conditionalFormatting sqref="D2:D33">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2356,7 +2408,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G32">
+  <conditionalFormatting sqref="G2:G33">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2364,17 +2416,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H32">
+  <conditionalFormatting sqref="H2:H33">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I32">
+  <conditionalFormatting sqref="I2:I33">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J32">
+  <conditionalFormatting sqref="J2:J33">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2389,7 +2441,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2469,6 +2521,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Klantenservice / Contact</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 18:24:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2387,8 +2387,60 @@
         </is>
       </c>
     </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Hebben we EcoPro-700 nog op voorraad?</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Testmail #6: Hebben we EcoPro-700 nog op voorraad?</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Inkoop / Bestellingen</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar inkoop@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>2025-08-03 18:23:53</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D33">
+  <conditionalFormatting sqref="D2:D34">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2408,7 +2460,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G33">
+  <conditionalFormatting sqref="G2:G34">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2416,17 +2468,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H33">
+  <conditionalFormatting sqref="H2:H34">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I33">
+  <conditionalFormatting sqref="I2:I34">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J33">
+  <conditionalFormatting sqref="J2:J34">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2498,7 +2550,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 18:26:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2439,8 +2439,60 @@
         </is>
       </c>
     </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Is dit artikel nog op voorraad?</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Testmail #7: Is dit artikel nog op voorraad?</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Inkoop / Bestellingen</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar inkoop@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>2025-08-03 18:26:21</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D34">
+  <conditionalFormatting sqref="D2:D35">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2460,7 +2512,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G34">
+  <conditionalFormatting sqref="G2:G35">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2468,17 +2520,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H34">
+  <conditionalFormatting sqref="H2:H35">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I34">
+  <conditionalFormatting sqref="I2:I35">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J34">
+  <conditionalFormatting sqref="J2:J35">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2536,17 +2588,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Intern verzoek / Actie voor medewerker</t>
+          <t>Inkoop / Bestellingen</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Inkoop / Bestellingen</t>
+          <t>Intern verzoek / Actie voor medewerker</t>
         </is>
       </c>
       <c r="B5" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 18:29:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2491,8 +2491,60 @@
         </is>
       </c>
     </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Kun je nagaan of dit nog leverbaar is?</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Testmail #8: Kun je nagaan of dit nog leverbaar is?</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Inkoop / Bestellingen</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar inkoop@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>2025-08-03 18:28:51</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D35">
+  <conditionalFormatting sqref="D2:D36">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2512,7 +2564,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G35">
+  <conditionalFormatting sqref="G2:G36">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2520,17 +2572,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H35">
+  <conditionalFormatting sqref="H2:H36">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I35">
+  <conditionalFormatting sqref="I2:I36">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J35">
+  <conditionalFormatting sqref="J2:J36">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2592,7 +2644,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 18:31:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2543,8 +2543,63 @@
         </is>
       </c>
     </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Hoi, hebben jullie al iets gehoord?</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Testmail #9: Hoi, hebben jullie al iets gehoord?</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Helaas kunnen we uw vraag niet beantwoorden omdat deze e-mail als een testmail is gemarkeerd. Mocht u een specifieke vraag hebben waarover wij u kunnen helpen, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Naam bedrijf]</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>2025-08-03 18:31:22</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D36">
+  <conditionalFormatting sqref="D2:D37">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2564,7 +2619,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G36">
+  <conditionalFormatting sqref="G2:G37">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2572,17 +2627,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H36">
+  <conditionalFormatting sqref="H2:H37">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I36">
+  <conditionalFormatting sqref="I2:I37">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J36">
+  <conditionalFormatting sqref="J2:J37">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2620,17 +2675,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Planning / Afspraak</t>
+          <t>Overig</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Overig</t>
+          <t>Planning / Afspraak</t>
         </is>
       </c>
       <c r="B3" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 18:33:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2598,8 +2598,64 @@
         </is>
       </c>
     </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Is er al nieuws?</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Testmail #10: Is er al nieuws?</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Beste afzender,
+Bedankt voor uw e-mail. Kunt u mij meer informatie geven over waar u precies naar op zoek bent? Op basis van uw vraag kan ik nu niet direct antwoorden met het juiste nieuws. Alvast bedankt voor uw aanvullende informatie.
+Met vriendelijke groet,
+[Naam] 
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>2025-08-03 18:33:40</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D37">
+  <conditionalFormatting sqref="D2:D38">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2619,7 +2675,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G37">
+  <conditionalFormatting sqref="G2:G38">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2627,17 +2683,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H37">
+  <conditionalFormatting sqref="H2:H38">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I37">
+  <conditionalFormatting sqref="I2:I38">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J37">
+  <conditionalFormatting sqref="J2:J38">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2679,7 +2735,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 18:36:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$8</f>
+              <f>'Dashboard'!$A$2:$A$9</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$8</f>
+              <f>'Dashboard'!$B$2:$B$9</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2654,8 +2654,63 @@
         </is>
       </c>
     </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Mijn retour is nog steeds niet verwerkt.</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Testmail #11: Mijn retour is nog steeds niet verwerkt.</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Dank u voor uw bericht. Kunt u ons meer informatie geven over uw retourzending, zoals uw ordernummer of retournummer, zodat we dit verder kunnen onderzoeken en u zo snel mogelijk kunnen helpen?
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>2025-08-03 18:35:51</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D38">
+  <conditionalFormatting sqref="D2:D39">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2675,7 +2730,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G38">
+  <conditionalFormatting sqref="G2:G39">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2683,17 +2738,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H38">
+  <conditionalFormatting sqref="H2:H39">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I38">
+  <conditionalFormatting sqref="I2:I39">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J38">
+  <conditionalFormatting sqref="J2:J39">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2708,7 +2763,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2798,6 +2853,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 18:38:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2709,8 +2709,64 @@
         </is>
       </c>
     </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Ik heb nog geen geld terug.</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Testmail #12: Ik heb nog geen geld terug.</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Dank u wel voor uw bericht. Om uw situatie te kunnen bekijken en u verder te kunnen helpen, hebben wij een aantal gegevens nodig. Kunt u ons alstublieft uw naam en het ordernummer doorgeven? Op die manier kunnen wij uw specifieke zaak onderzoeken en nagaan waarom het terugbetalingsproces nog niet is afgerond.
+Wij kijken uit naar uw reactie.
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>2025-08-03 18:38:04</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D39">
+  <conditionalFormatting sqref="D2:D40">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2730,7 +2786,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G39">
+  <conditionalFormatting sqref="G2:G40">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2738,17 +2794,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H39">
+  <conditionalFormatting sqref="H2:H40">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I39">
+  <conditionalFormatting sqref="I2:I40">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J39">
+  <conditionalFormatting sqref="J2:J40">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2826,17 +2882,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Documentatie / Datasheets</t>
+          <t>Retour / Terugbetaling</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Klacht / Probleem</t>
+          <t>Documentatie / Datasheets</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -2846,7 +2902,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Klantenservice / Contact</t>
+          <t>Klacht / Probleem</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -2856,7 +2912,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Retour / Terugbetaling</t>
+          <t>Klantenservice / Contact</t>
         </is>
       </c>
       <c r="B9" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 18:40:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2765,8 +2765,60 @@
         </is>
       </c>
     </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Kun je mij de datasheet van de VentiQ-250 sturen?</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Testmail #13: Kun je mij de datasheet van de VentiQ-250 sturen?</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Documentatie / Datasheets</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar documentatie@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>2025-08-03 18:40:14</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D40">
+  <conditionalFormatting sqref="D2:D41">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2786,7 +2838,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G40">
+  <conditionalFormatting sqref="G2:G41">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2794,17 +2846,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H40">
+  <conditionalFormatting sqref="H2:H41">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I40">
+  <conditionalFormatting sqref="I2:I41">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J40">
+  <conditionalFormatting sqref="J2:J41">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2882,7 +2934,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Retour / Terugbetaling</t>
+          <t>Documentatie / Datasheets</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -2892,11 +2944,11 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Documentatie / Datasheets</t>
+          <t>Retour / Terugbetaling</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 18:42:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$9</f>
+              <f>'Dashboard'!$A$2:$A$10</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$9</f>
+              <f>'Dashboard'!$B$2:$B$10</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2817,8 +2817,60 @@
         </is>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Heb je de CE-certificaten van dit product?</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Testmail #14: Heb je de CE-certificaten van dit product?</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Kwaliteit / Certificaten</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar kwaliteit@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>2025-08-03 18:42:24</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D41">
+  <conditionalFormatting sqref="D2:D42">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2838,7 +2890,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G41">
+  <conditionalFormatting sqref="G2:G42">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2846,17 +2898,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H41">
+  <conditionalFormatting sqref="H2:H42">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I41">
+  <conditionalFormatting sqref="I2:I42">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J41">
+  <conditionalFormatting sqref="J2:J42">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2871,7 +2923,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2971,6 +3023,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Kwaliteit / Certificaten</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 18:44:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2869,8 +2869,60 @@
         </is>
       </c>
     </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Leg dit even neer bij Koen.</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Testmail #15: Leg dit even neer bij Koen.</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>2025-08-03 18:44:33</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D42">
+  <conditionalFormatting sqref="D2:D43">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2890,7 +2942,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G42">
+  <conditionalFormatting sqref="G2:G43">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2898,17 +2950,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H42">
+  <conditionalFormatting sqref="H2:H43">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I42">
+  <conditionalFormatting sqref="I2:I43">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J42">
+  <conditionalFormatting sqref="J2:J43">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2960,7 +3012,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 18:46:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J43"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2921,8 +2921,60 @@
         </is>
       </c>
     </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Wil je dit even doorsturen?</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Testmail #16: Wil je dit even doorsturen?</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>2025-08-03 18:46:43</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D43">
+  <conditionalFormatting sqref="D2:D44">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2942,7 +2994,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G43">
+  <conditionalFormatting sqref="G2:G44">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2950,17 +3002,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H43">
+  <conditionalFormatting sqref="H2:H44">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I43">
+  <conditionalFormatting sqref="I2:I44">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J43">
+  <conditionalFormatting sqref="J2:J44">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2998,7 +3050,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Overig</t>
+          <t>Planning / Afspraak</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -3008,11 +3060,11 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Planning / Afspraak</t>
+          <t>Overig</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 18:49:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2973,8 +2973,60 @@
         </is>
       </c>
     </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Testmail #17: Kun je vrijdag om 11:00 een demo inplannen bij Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>2025-08-03 18:48:56</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D44">
+  <conditionalFormatting sqref="D2:D45">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2994,7 +3046,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G44">
+  <conditionalFormatting sqref="G2:G45">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3002,17 +3054,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H44">
+  <conditionalFormatting sqref="H2:H45">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I44">
+  <conditionalFormatting sqref="I2:I45">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J44">
+  <conditionalFormatting sqref="J2:J45">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3054,7 +3106,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 18:51:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3025,8 +3025,60 @@
         </is>
       </c>
     </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Bestel je 200 stuks M8-bouten RVS voor Van Dijk?</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Testmail #18: Bestel je 200 stuks M8-bouten RVS voor Van Dijk?</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Inkoop / Bestellingen</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar inkoop@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>2025-08-03 18:51:06</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D45">
+  <conditionalFormatting sqref="D2:D46">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -3046,7 +3098,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G45">
+  <conditionalFormatting sqref="G2:G46">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3054,17 +3106,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H45">
+  <conditionalFormatting sqref="H2:H46">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I45">
+  <conditionalFormatting sqref="I2:I46">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J45">
+  <conditionalFormatting sqref="J2:J46">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3126,7 +3178,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 18:53:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3077,8 +3077,60 @@
         </is>
       </c>
     </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Bel jij klant Jansen even?</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Testmail #19: Bel jij klant Jansen even?</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Klantenservice / Contact</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar klantenservice@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>2025-08-03 18:53:19</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D46">
+  <conditionalFormatting sqref="D2:D47">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -3098,7 +3150,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G46">
+  <conditionalFormatting sqref="G2:G47">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3106,17 +3158,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H46">
+  <conditionalFormatting sqref="H2:H47">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I46">
+  <conditionalFormatting sqref="I2:I47">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J46">
+  <conditionalFormatting sqref="J2:J47">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3204,7 +3256,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Retour / Terugbetaling</t>
+          <t>Klantenservice / Contact</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -3214,17 +3266,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Klacht / Probleem</t>
+          <t>Retour / Terugbetaling</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Klantenservice / Contact</t>
+          <t>Klacht / Probleem</t>
         </is>
       </c>
       <c r="B9" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 18:55:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J47"/>
+  <dimension ref="A1:J48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3129,8 +3129,60 @@
         </is>
       </c>
     </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Ik ben niet tevreden over hoe dit is gegaan.</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Testmail #20: Ik ben niet tevreden over hoe dit is gegaan.</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Klacht / Probleem</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar klachten@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>2025-08-03 18:55:27</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D47">
+  <conditionalFormatting sqref="D2:D48">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -3150,7 +3202,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G47">
+  <conditionalFormatting sqref="G2:G48">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3158,17 +3210,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H47">
+  <conditionalFormatting sqref="H2:H48">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I47">
+  <conditionalFormatting sqref="I2:I48">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J47">
+  <conditionalFormatting sqref="J2:J48">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3256,7 +3308,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Klantenservice / Contact</t>
+          <t>Klacht / Probleem</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -3266,7 +3318,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Retour / Terugbetaling</t>
+          <t>Klantenservice / Contact</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -3276,11 +3328,11 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Klacht / Probleem</t>
+          <t>Retour / Terugbetaling</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 23:16:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J48"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3181,8 +3181,60 @@
         </is>
       </c>
     </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Kun jij dit afhandelen?</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Testmail #1: Kun jij dit afhandelen?</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>2025-08-03 23:16:03</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D48">
+  <conditionalFormatting sqref="D2:D49">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -3202,7 +3254,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G48">
+  <conditionalFormatting sqref="G2:G49">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3210,17 +3262,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H48">
+  <conditionalFormatting sqref="H2:H49">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I48">
+  <conditionalFormatting sqref="I2:I49">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J48">
+  <conditionalFormatting sqref="J2:J49">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3262,7 +3314,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 23:26:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J49"/>
+  <dimension ref="A1:J50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3233,8 +3233,60 @@
         </is>
       </c>
     </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Kun jij dit afhandelen?</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Testmail #1: Kun jij dit afhandelen?</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>2025-08-03 23:26:42</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D49">
+  <conditionalFormatting sqref="D2:D50">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -3254,7 +3306,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G49">
+  <conditionalFormatting sqref="G2:G50">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3262,17 +3314,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H49">
+  <conditionalFormatting sqref="H2:H50">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I49">
+  <conditionalFormatting sqref="I2:I50">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J49">
+  <conditionalFormatting sqref="J2:J50">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3314,7 +3366,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 23:29:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3285,8 +3285,60 @@
         </is>
       </c>
     </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Wil je 100 stuks M5-bouten bestellen?</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Testmail #2: Wil je 100 stuks M5-bouten bestellen?</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Inkoop / Bestellingen</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar inkoop@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>2025-08-03 23:28:53</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D50">
+  <conditionalFormatting sqref="D2:D51">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -3306,7 +3358,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G50">
+  <conditionalFormatting sqref="G2:G51">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3314,17 +3366,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H50">
+  <conditionalFormatting sqref="H2:H51">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I50">
+  <conditionalFormatting sqref="I2:I51">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J50">
+  <conditionalFormatting sqref="J2:J51">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3386,7 +3438,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 23:31:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J51"/>
+  <dimension ref="A1:J52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3337,8 +3337,60 @@
         </is>
       </c>
     </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Hoi, hebben jullie al iets gehoord?</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Testmail #3: Hoi, hebben jullie al iets gehoord?</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar support@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>2025-08-03 23:31:12</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D51">
+  <conditionalFormatting sqref="D2:D52">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -3358,7 +3410,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G51">
+  <conditionalFormatting sqref="G2:G52">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3366,17 +3418,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H51">
+  <conditionalFormatting sqref="H2:H52">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I51">
+  <conditionalFormatting sqref="I2:I52">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J51">
+  <conditionalFormatting sqref="J2:J52">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3428,7 +3480,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 23:33:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J52"/>
+  <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3389,8 +3389,60 @@
         </is>
       </c>
     </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Is er al nieuws?</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Testmail #4: Is er al nieuws?</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar support@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>2025-08-03 23:33:43</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D52">
+  <conditionalFormatting sqref="D2:D53">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -3410,7 +3462,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G52">
+  <conditionalFormatting sqref="G2:G53">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3418,17 +3470,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H52">
+  <conditionalFormatting sqref="H2:H53">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I52">
+  <conditionalFormatting sqref="I2:I53">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J52">
+  <conditionalFormatting sqref="J2:J53">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3480,7 +3532,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-03 23:36:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-03.xlsx
+++ b/logs/mail_log_2025-08-03.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J53"/>
+  <dimension ref="A1:J54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3441,8 +3441,64 @@
         </is>
       </c>
     </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Ik heb nog geen geld terug.</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Testmail #5: Ik heb nog geen geld terug.</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Hartelijk dank voor uw bericht. Kunt u mij het volgende laten weten: om welke aankoop gaat het precies en wanneer heeft u deze gedaan? Op basis van die informatie kunnen we de status van uw terugbetaling controleren en u verder helpen.
+Met vriendelijke groet,  
+[Naam]  
+Klantenservice Team</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>2025-08-03 23:35:55</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D53">
+  <conditionalFormatting sqref="D2:D54">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -3462,7 +3518,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G53">
+  <conditionalFormatting sqref="G2:G54">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3470,17 +3526,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H53">
+  <conditionalFormatting sqref="H2:H54">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I53">
+  <conditionalFormatting sqref="I2:I54">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J53">
+  <conditionalFormatting sqref="J2:J54">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3558,17 +3614,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Documentatie / Datasheets</t>
+          <t>Retour / Terugbetaling</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Klacht / Probleem</t>
+          <t>Documentatie / Datasheets</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -3578,7 +3634,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Klantenservice / Contact</t>
+          <t>Klacht / Probleem</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -3588,7 +3644,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Retour / Terugbetaling</t>
+          <t>Klantenservice / Contact</t>
         </is>
       </c>
       <c r="B9" t="n">

</xml_diff>